<commit_message>
Updated device definitions Excel templates to include the field for the meter's name.
</commit_message>
<xml_diff>
--- a/Source/Documentation/Device Definitions Examples & Templates/openXDA Configuration Template - DFR.xlsx
+++ b/Source/Documentation/Device Definitions Examples & Templates/openXDA Configuration Template - DFR.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17030"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17329"/>
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="S:\Products\openXDA\Documentation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\openXDA\Source\Documentation\Device Definitions Examples &amp; Templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="63">
   <si>
     <t>USE</t>
   </si>
@@ -147,19 +147,10 @@
     <t>stationLongitude</t>
   </si>
   <si>
-    <t>This template is intended for use in configuring an openXDA database for data from substation devices such as digital fault recorders; one device per template. A separate template is available for PQ monitors and relays. Each device must be defined by specifying the information described below. Please enter a value for each parameter. "ID" fields are limited to 50 alphanumeric characters, other non-numeric fields can contain up to 200 alphanumeric characters.</t>
-  </si>
-  <si>
     <t>Your Value</t>
   </si>
   <si>
     <t>Parameter Description</t>
-  </si>
-  <si>
-    <t>Unique ID for the location of the device: Up to 50 alphanumeric characters.</t>
-  </si>
-  <si>
-    <t>Human readable name for the location: Up to 200 alphanumeric characters.</t>
   </si>
   <si>
     <t>Numeric decimal value</t>
@@ -197,9 +188,6 @@
     </r>
   </si>
   <si>
-    <t>Human readable name for the line or location: Up to 200 alphanumeric characters.</t>
-  </si>
-  <si>
     <r>
       <t>Nominal voltage in</t>
     </r>
@@ -250,13 +238,28 @@
     <t>As a general rule, the device id is the name of the folder where the data is stored for that device. DFR data should be in COMTRADE or native E-Max format.</t>
   </si>
   <si>
-    <t>Specific information about the reporting device; DFR etc. Up to 200 alphanumeric characters each for make and model fields.</t>
-  </si>
-  <si>
     <t>If a device is monitoring more than one line, please copy the section outlined in blue and paste it below, then fill in the appropriate information.</t>
   </si>
   <si>
     <t xml:space="preserve">Channel definitions are only required for COMTRADE input files. </t>
+  </si>
+  <si>
+    <t>Specific information about the reporting device; DFR etc. Up to 200 characters each for make and model fields.</t>
+  </si>
+  <si>
+    <t>Unique ID for the location of the device: Up to 50 characters.</t>
+  </si>
+  <si>
+    <t>Human readable name for the location: Up to 200 characters.</t>
+  </si>
+  <si>
+    <t>Human readable name for the reporting device; DFR etc. Up to 200 characters.</t>
+  </si>
+  <si>
+    <t>Human readable name for the line or location: Up to 200 characters.</t>
+  </si>
+  <si>
+    <t>This template is intended for use in configuring an openXDA database for data from substation devices such as digital fault recorders; one device per template. A separate template is available for PQ monitors and relays. Each device must be defined by specifying the information described below. Please enter a value for each parameter. "ID" fields are limited to 50 characters, other non-numeric fields can contain up to 200 characters.</t>
   </si>
 </sst>
 </file>
@@ -1041,6 +1044,64 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="18" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="21" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="32" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="36" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="37" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="43" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="42" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="45" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="49" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="50" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="51" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="52" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="53" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="52" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="54" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -1052,44 +1113,104 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="38" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="38" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="40" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
@@ -1100,32 +1221,6 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="18" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="21" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -1135,109 +1230,17 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="46" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="47" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="48" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="32" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="36" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="37" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="38" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="40" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="38" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="43" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="42" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="45" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="44" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="46" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="47" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="48" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="49" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="50" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="51" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="52" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="53" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="52" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="54" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -1571,45 +1574,45 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A1" s="12" t="s">
+      <c r="A1" s="42" t="s">
         <v>35</v>
       </c>
-      <c r="B1" s="13"/>
-      <c r="C1" s="13"/>
-      <c r="D1" s="13"/>
-      <c r="E1" s="13"/>
-      <c r="F1" s="13"/>
-      <c r="G1" s="13"/>
-      <c r="H1" s="13"/>
-      <c r="I1" s="13"/>
-      <c r="J1" s="13"/>
-      <c r="K1" s="14"/>
+      <c r="B1" s="43"/>
+      <c r="C1" s="43"/>
+      <c r="D1" s="43"/>
+      <c r="E1" s="43"/>
+      <c r="F1" s="43"/>
+      <c r="G1" s="43"/>
+      <c r="H1" s="43"/>
+      <c r="I1" s="43"/>
+      <c r="J1" s="43"/>
+      <c r="K1" s="44"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A2" s="15"/>
-      <c r="B2" s="16"/>
-      <c r="C2" s="16"/>
-      <c r="D2" s="16"/>
-      <c r="E2" s="16"/>
-      <c r="F2" s="16"/>
-      <c r="G2" s="16"/>
-      <c r="H2" s="16"/>
-      <c r="I2" s="16"/>
-      <c r="J2" s="16"/>
-      <c r="K2" s="17"/>
+      <c r="A2" s="45"/>
+      <c r="B2" s="46"/>
+      <c r="C2" s="46"/>
+      <c r="D2" s="46"/>
+      <c r="E2" s="46"/>
+      <c r="F2" s="46"/>
+      <c r="G2" s="46"/>
+      <c r="H2" s="46"/>
+      <c r="I2" s="46"/>
+      <c r="J2" s="46"/>
+      <c r="K2" s="47"/>
     </row>
     <row r="3" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="18"/>
-      <c r="B3" s="19"/>
-      <c r="C3" s="19"/>
-      <c r="D3" s="19"/>
-      <c r="E3" s="19"/>
-      <c r="F3" s="19"/>
-      <c r="G3" s="19"/>
-      <c r="H3" s="19"/>
-      <c r="I3" s="19"/>
-      <c r="J3" s="19"/>
-      <c r="K3" s="20"/>
+      <c r="A3" s="48"/>
+      <c r="B3" s="49"/>
+      <c r="C3" s="49"/>
+      <c r="D3" s="49"/>
+      <c r="E3" s="49"/>
+      <c r="F3" s="49"/>
+      <c r="G3" s="49"/>
+      <c r="H3" s="49"/>
+      <c r="I3" s="49"/>
+      <c r="J3" s="49"/>
+      <c r="K3" s="50"/>
     </row>
     <row r="4" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="5" spans="1:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -1676,10 +1679,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M43"/>
+  <dimension ref="A1:M44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="M28" sqref="M28"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:K4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1690,58 +1693,58 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="22" t="s">
-        <v>40</v>
-      </c>
-      <c r="B1" s="23"/>
-      <c r="C1" s="23"/>
-      <c r="D1" s="23"/>
-      <c r="E1" s="23"/>
-      <c r="F1" s="23"/>
-      <c r="G1" s="23"/>
-      <c r="H1" s="23"/>
-      <c r="I1" s="23"/>
-      <c r="J1" s="23"/>
-      <c r="K1" s="24"/>
+      <c r="A1" s="63" t="s">
+        <v>62</v>
+      </c>
+      <c r="B1" s="64"/>
+      <c r="C1" s="64"/>
+      <c r="D1" s="64"/>
+      <c r="E1" s="64"/>
+      <c r="F1" s="64"/>
+      <c r="G1" s="64"/>
+      <c r="H1" s="64"/>
+      <c r="I1" s="64"/>
+      <c r="J1" s="64"/>
+      <c r="K1" s="65"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A2" s="25"/>
-      <c r="B2" s="26"/>
-      <c r="C2" s="26"/>
-      <c r="D2" s="26"/>
-      <c r="E2" s="26"/>
-      <c r="F2" s="26"/>
-      <c r="G2" s="26"/>
-      <c r="H2" s="26"/>
-      <c r="I2" s="26"/>
-      <c r="J2" s="26"/>
-      <c r="K2" s="27"/>
+      <c r="A2" s="66"/>
+      <c r="B2" s="67"/>
+      <c r="C2" s="67"/>
+      <c r="D2" s="67"/>
+      <c r="E2" s="67"/>
+      <c r="F2" s="67"/>
+      <c r="G2" s="67"/>
+      <c r="H2" s="67"/>
+      <c r="I2" s="67"/>
+      <c r="J2" s="67"/>
+      <c r="K2" s="68"/>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A3" s="25"/>
-      <c r="B3" s="26"/>
-      <c r="C3" s="26"/>
-      <c r="D3" s="26"/>
-      <c r="E3" s="26"/>
-      <c r="F3" s="26"/>
-      <c r="G3" s="26"/>
-      <c r="H3" s="26"/>
-      <c r="I3" s="26"/>
-      <c r="J3" s="26"/>
-      <c r="K3" s="27"/>
+      <c r="A3" s="66"/>
+      <c r="B3" s="67"/>
+      <c r="C3" s="67"/>
+      <c r="D3" s="67"/>
+      <c r="E3" s="67"/>
+      <c r="F3" s="67"/>
+      <c r="G3" s="67"/>
+      <c r="H3" s="67"/>
+      <c r="I3" s="67"/>
+      <c r="J3" s="67"/>
+      <c r="K3" s="68"/>
     </row>
     <row r="4" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="28"/>
-      <c r="B4" s="29"/>
-      <c r="C4" s="29"/>
-      <c r="D4" s="29"/>
-      <c r="E4" s="29"/>
-      <c r="F4" s="29"/>
-      <c r="G4" s="29"/>
-      <c r="H4" s="29"/>
-      <c r="I4" s="29"/>
-      <c r="J4" s="29"/>
-      <c r="K4" s="30"/>
+      <c r="A4" s="69"/>
+      <c r="B4" s="70"/>
+      <c r="C4" s="70"/>
+      <c r="D4" s="70"/>
+      <c r="E4" s="70"/>
+      <c r="F4" s="70"/>
+      <c r="G4" s="70"/>
+      <c r="H4" s="70"/>
+      <c r="I4" s="70"/>
+      <c r="J4" s="70"/>
+      <c r="K4" s="71"/>
     </row>
     <row r="5" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="6" spans="1:11" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -1749,53 +1752,53 @@
         <v>8</v>
       </c>
       <c r="B6" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="C6" s="84" t="s">
         <v>41</v>
       </c>
-      <c r="C6" s="34" t="s">
-        <v>42</v>
-      </c>
-      <c r="D6" s="35"/>
-      <c r="E6" s="35"/>
-      <c r="F6" s="35"/>
-      <c r="G6" s="35"/>
-      <c r="H6" s="35"/>
-      <c r="I6" s="35"/>
-      <c r="J6" s="35"/>
-      <c r="K6" s="36"/>
+      <c r="D6" s="85"/>
+      <c r="E6" s="85"/>
+      <c r="F6" s="85"/>
+      <c r="G6" s="85"/>
+      <c r="H6" s="85"/>
+      <c r="I6" s="85"/>
+      <c r="J6" s="85"/>
+      <c r="K6" s="86"/>
     </row>
     <row r="7" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
         <v>11</v>
       </c>
       <c r="B7" s="11"/>
-      <c r="C7" s="37" t="s">
-        <v>58</v>
-      </c>
-      <c r="D7" s="37"/>
-      <c r="E7" s="37"/>
-      <c r="F7" s="37"/>
-      <c r="G7" s="37"/>
-      <c r="H7" s="37"/>
-      <c r="I7" s="37"/>
-      <c r="J7" s="37"/>
-      <c r="K7" s="37"/>
+      <c r="C7" s="72" t="s">
+        <v>54</v>
+      </c>
+      <c r="D7" s="72"/>
+      <c r="E7" s="72"/>
+      <c r="F7" s="72"/>
+      <c r="G7" s="72"/>
+      <c r="H7" s="72"/>
+      <c r="I7" s="72"/>
+      <c r="J7" s="72"/>
+      <c r="K7" s="72"/>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="8"/>
       <c r="B8" s="8"/>
-      <c r="C8" s="31"/>
-      <c r="D8" s="31"/>
-      <c r="E8" s="31"/>
-      <c r="F8" s="31"/>
-      <c r="G8" s="31"/>
-      <c r="H8" s="31"/>
-      <c r="I8" s="31"/>
-      <c r="J8" s="31"/>
-      <c r="K8" s="31"/>
+      <c r="C8" s="73"/>
+      <c r="D8" s="73"/>
+      <c r="E8" s="73"/>
+      <c r="F8" s="73"/>
+      <c r="G8" s="73"/>
+      <c r="H8" s="73"/>
+      <c r="I8" s="73"/>
+      <c r="J8" s="73"/>
+      <c r="K8" s="73"/>
     </row>
     <row r="9" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="10" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="38" t="s">
+      <c r="A10" s="12" t="s">
         <v>9</v>
       </c>
       <c r="B10" s="6"/>
@@ -1809,553 +1812,571 @@
       <c r="J10" s="6"/>
       <c r="K10" s="6"/>
     </row>
-    <row r="11" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="39" t="s">
+    <row r="11" spans="1:11" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="B11" s="14"/>
+      <c r="C11" s="74" t="s">
+        <v>60</v>
+      </c>
+      <c r="D11" s="74"/>
+      <c r="E11" s="74"/>
+      <c r="F11" s="74"/>
+      <c r="G11" s="74"/>
+      <c r="H11" s="74"/>
+      <c r="I11" s="74"/>
+      <c r="J11" s="74"/>
+      <c r="K11" s="75"/>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A12" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="B11" s="40"/>
-      <c r="C11" s="41" t="s">
+      <c r="B12" s="14"/>
+      <c r="C12" s="74" t="s">
+        <v>57</v>
+      </c>
+      <c r="D12" s="74"/>
+      <c r="E12" s="74"/>
+      <c r="F12" s="74"/>
+      <c r="G12" s="74"/>
+      <c r="H12" s="74"/>
+      <c r="I12" s="74"/>
+      <c r="J12" s="74"/>
+      <c r="K12" s="75"/>
+    </row>
+    <row r="13" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="B13" s="16"/>
+      <c r="C13" s="76"/>
+      <c r="D13" s="76"/>
+      <c r="E13" s="76"/>
+      <c r="F13" s="76"/>
+      <c r="G13" s="76"/>
+      <c r="H13" s="76"/>
+      <c r="I13" s="76"/>
+      <c r="J13" s="76"/>
+      <c r="K13" s="77"/>
+    </row>
+    <row r="14" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="B14" s="14"/>
+      <c r="C14" s="87" t="s">
+        <v>58</v>
+      </c>
+      <c r="D14" s="88"/>
+      <c r="E14" s="88"/>
+      <c r="F14" s="88"/>
+      <c r="G14" s="88"/>
+      <c r="H14" s="88"/>
+      <c r="I14" s="88"/>
+      <c r="J14" s="88"/>
+      <c r="K14" s="89"/>
+    </row>
+    <row r="15" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="17" t="s">
+        <v>20</v>
+      </c>
+      <c r="B15" s="11"/>
+      <c r="C15" s="51" t="s">
         <v>59</v>
       </c>
-      <c r="D11" s="41"/>
-      <c r="E11" s="41"/>
-      <c r="F11" s="41"/>
-      <c r="G11" s="41"/>
-      <c r="H11" s="41"/>
-      <c r="I11" s="41"/>
-      <c r="J11" s="41"/>
-      <c r="K11" s="42"/>
-    </row>
-    <row r="12" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="43" t="s">
-        <v>18</v>
-      </c>
-      <c r="B12" s="44"/>
-      <c r="C12" s="45"/>
-      <c r="D12" s="45"/>
-      <c r="E12" s="45"/>
-      <c r="F12" s="45"/>
-      <c r="G12" s="45"/>
-      <c r="H12" s="45"/>
-      <c r="I12" s="45"/>
-      <c r="J12" s="45"/>
-      <c r="K12" s="46"/>
-    </row>
-    <row r="13" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="39" t="s">
-        <v>19</v>
-      </c>
-      <c r="B13" s="40"/>
-      <c r="C13" s="47" t="s">
+      <c r="D15" s="52"/>
+      <c r="E15" s="52"/>
+      <c r="F15" s="52"/>
+      <c r="G15" s="52"/>
+      <c r="H15" s="52"/>
+      <c r="I15" s="52"/>
+      <c r="J15" s="52"/>
+      <c r="K15" s="53"/>
+    </row>
+    <row r="16" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="18" t="s">
+        <v>38</v>
+      </c>
+      <c r="B16" s="11"/>
+      <c r="C16" s="51" t="s">
+        <v>42</v>
+      </c>
+      <c r="D16" s="52"/>
+      <c r="E16" s="52"/>
+      <c r="F16" s="52"/>
+      <c r="G16" s="52"/>
+      <c r="H16" s="52"/>
+      <c r="I16" s="52"/>
+      <c r="J16" s="52"/>
+      <c r="K16" s="53"/>
+    </row>
+    <row r="17" spans="1:13" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="19" t="s">
+        <v>39</v>
+      </c>
+      <c r="B17" s="16"/>
+      <c r="C17" s="54" t="s">
+        <v>42</v>
+      </c>
+      <c r="D17" s="55"/>
+      <c r="E17" s="55"/>
+      <c r="F17" s="55"/>
+      <c r="G17" s="55"/>
+      <c r="H17" s="55"/>
+      <c r="I17" s="55"/>
+      <c r="J17" s="55"/>
+      <c r="K17" s="56"/>
+    </row>
+    <row r="18" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="35"/>
+      <c r="C18" s="25"/>
+    </row>
+    <row r="19" spans="1:13" ht="15.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="36" t="s">
         <v>43</v>
       </c>
-      <c r="D13" s="48"/>
-      <c r="E13" s="48"/>
-      <c r="F13" s="48"/>
-      <c r="G13" s="48"/>
-      <c r="H13" s="48"/>
-      <c r="I13" s="48"/>
-      <c r="J13" s="48"/>
-      <c r="K13" s="49"/>
-    </row>
-    <row r="14" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="50" t="s">
-        <v>20</v>
-      </c>
-      <c r="B14" s="11"/>
-      <c r="C14" s="33" t="s">
+      <c r="B19" s="24"/>
+      <c r="C19" s="57" t="s">
         <v>44</v>
       </c>
-      <c r="D14" s="51"/>
-      <c r="E14" s="51"/>
-      <c r="F14" s="51"/>
-      <c r="G14" s="51"/>
-      <c r="H14" s="51"/>
-      <c r="I14" s="51"/>
-      <c r="J14" s="51"/>
-      <c r="K14" s="52"/>
-    </row>
-    <row r="15" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="53" t="s">
-        <v>38</v>
-      </c>
-      <c r="B15" s="11"/>
-      <c r="C15" s="33" t="s">
+      <c r="D19" s="58"/>
+      <c r="E19" s="58"/>
+      <c r="F19" s="58"/>
+      <c r="G19" s="58"/>
+      <c r="H19" s="58"/>
+      <c r="I19" s="58"/>
+      <c r="J19" s="58"/>
+      <c r="K19" s="59"/>
+      <c r="L19" s="28"/>
+      <c r="M19" s="20"/>
+    </row>
+    <row r="20" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="37" t="s">
+        <v>10</v>
+      </c>
+      <c r="B20" s="11"/>
+      <c r="C20" s="78" t="s">
         <v>45</v>
       </c>
-      <c r="D15" s="51"/>
-      <c r="E15" s="51"/>
-      <c r="F15" s="51"/>
-      <c r="G15" s="51"/>
-      <c r="H15" s="51"/>
-      <c r="I15" s="51"/>
-      <c r="J15" s="51"/>
-      <c r="K15" s="52"/>
-    </row>
-    <row r="16" spans="1:11" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="54" t="s">
-        <v>39</v>
-      </c>
-      <c r="B16" s="44"/>
-      <c r="C16" s="55" t="s">
-        <v>45</v>
-      </c>
-      <c r="D16" s="56"/>
-      <c r="E16" s="56"/>
-      <c r="F16" s="56"/>
-      <c r="G16" s="56"/>
-      <c r="H16" s="56"/>
-      <c r="I16" s="56"/>
-      <c r="J16" s="56"/>
-      <c r="K16" s="57"/>
-    </row>
-    <row r="17" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="87"/>
-      <c r="C17" s="66"/>
-    </row>
-    <row r="18" spans="1:13" ht="15.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="88" t="s">
+      <c r="D20" s="78"/>
+      <c r="E20" s="78"/>
+      <c r="F20" s="78"/>
+      <c r="G20" s="78"/>
+      <c r="H20" s="78"/>
+      <c r="I20" s="78"/>
+      <c r="J20" s="78"/>
+      <c r="K20" s="79"/>
+      <c r="L20" s="27"/>
+      <c r="M20" s="20"/>
+    </row>
+    <row r="21" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="38" t="s">
+        <v>12</v>
+      </c>
+      <c r="B21" s="11"/>
+      <c r="C21" s="80" t="s">
+        <v>61</v>
+      </c>
+      <c r="D21" s="80"/>
+      <c r="E21" s="80"/>
+      <c r="F21" s="80"/>
+      <c r="G21" s="80"/>
+      <c r="H21" s="80"/>
+      <c r="I21" s="80"/>
+      <c r="J21" s="80"/>
+      <c r="K21" s="81"/>
+      <c r="L21" s="27"/>
+      <c r="M21" s="20"/>
+    </row>
+    <row r="22" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="38" t="s">
+        <v>13</v>
+      </c>
+      <c r="B22" s="11"/>
+      <c r="C22" s="80" t="s">
         <v>46</v>
       </c>
-      <c r="B18" s="65"/>
-      <c r="C18" s="67" t="s">
+      <c r="D22" s="80"/>
+      <c r="E22" s="80"/>
+      <c r="F22" s="80"/>
+      <c r="G22" s="80"/>
+      <c r="H22" s="80"/>
+      <c r="I22" s="80"/>
+      <c r="J22" s="80"/>
+      <c r="K22" s="81"/>
+      <c r="L22" s="27"/>
+    </row>
+    <row r="23" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="39" t="s">
+        <v>14</v>
+      </c>
+      <c r="B23" s="23"/>
+      <c r="C23" s="82" t="s">
         <v>47</v>
       </c>
-      <c r="D18" s="68"/>
-      <c r="E18" s="68"/>
-      <c r="F18" s="68"/>
-      <c r="G18" s="68"/>
-      <c r="H18" s="68"/>
-      <c r="I18" s="68"/>
-      <c r="J18" s="68"/>
-      <c r="K18" s="77"/>
-      <c r="L18" s="71"/>
-      <c r="M18" s="58"/>
-    </row>
-    <row r="19" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="89" t="s">
-        <v>10</v>
-      </c>
-      <c r="B19" s="11"/>
-      <c r="C19" s="32" t="s">
+      <c r="D23" s="82"/>
+      <c r="E23" s="82"/>
+      <c r="F23" s="82"/>
+      <c r="G23" s="82"/>
+      <c r="H23" s="82"/>
+      <c r="I23" s="82"/>
+      <c r="J23" s="82"/>
+      <c r="K23" s="83"/>
+      <c r="L23" s="27"/>
+    </row>
+    <row r="24" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="38" t="s">
+        <v>15</v>
+      </c>
+      <c r="B24" s="11"/>
+      <c r="C24" s="80" t="s">
         <v>48</v>
       </c>
-      <c r="D19" s="32"/>
-      <c r="E19" s="32"/>
-      <c r="F19" s="32"/>
-      <c r="G19" s="32"/>
-      <c r="H19" s="32"/>
-      <c r="I19" s="32"/>
-      <c r="J19" s="32"/>
-      <c r="K19" s="78"/>
-      <c r="L19" s="70"/>
-      <c r="M19" s="58"/>
-    </row>
-    <row r="20" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="90" t="s">
-        <v>12</v>
-      </c>
-      <c r="B20" s="11"/>
-      <c r="C20" s="21" t="s">
+      <c r="D24" s="80"/>
+      <c r="E24" s="80"/>
+      <c r="F24" s="80"/>
+      <c r="G24" s="80"/>
+      <c r="H24" s="80"/>
+      <c r="I24" s="80"/>
+      <c r="J24" s="80"/>
+      <c r="K24" s="81"/>
+      <c r="L24" s="27"/>
+    </row>
+    <row r="25" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="38" t="s">
+        <v>16</v>
+      </c>
+      <c r="B25" s="11"/>
+      <c r="C25" s="80" t="s">
         <v>49</v>
       </c>
-      <c r="D20" s="21"/>
-      <c r="E20" s="21"/>
-      <c r="F20" s="21"/>
-      <c r="G20" s="21"/>
-      <c r="H20" s="21"/>
-      <c r="I20" s="21"/>
-      <c r="J20" s="21"/>
-      <c r="K20" s="73"/>
-      <c r="L20" s="70"/>
-      <c r="M20" s="58"/>
-    </row>
-    <row r="21" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="90" t="s">
-        <v>13</v>
-      </c>
-      <c r="B21" s="11"/>
-      <c r="C21" s="21" t="s">
+      <c r="D25" s="80"/>
+      <c r="E25" s="80"/>
+      <c r="F25" s="80"/>
+      <c r="G25" s="80"/>
+      <c r="H25" s="80"/>
+      <c r="I25" s="80"/>
+      <c r="J25" s="80"/>
+      <c r="K25" s="81"/>
+      <c r="L25" s="27"/>
+    </row>
+    <row r="26" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="40"/>
+      <c r="B26" s="20"/>
+      <c r="C26" s="21"/>
+      <c r="D26" s="21"/>
+      <c r="E26" s="21"/>
+      <c r="F26" s="21"/>
+      <c r="G26" s="21"/>
+      <c r="H26" s="21"/>
+      <c r="I26" s="21"/>
+      <c r="J26" s="21"/>
+      <c r="K26" s="30"/>
+      <c r="L26" s="27"/>
+    </row>
+    <row r="27" spans="1:13" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="41" t="s">
+        <v>21</v>
+      </c>
+      <c r="B27" s="22"/>
+      <c r="C27" s="60" t="s">
+        <v>36</v>
+      </c>
+      <c r="D27" s="61"/>
+      <c r="E27" s="61"/>
+      <c r="F27" s="61"/>
+      <c r="G27" s="61"/>
+      <c r="H27" s="61"/>
+      <c r="I27" s="61"/>
+      <c r="J27" s="61"/>
+      <c r="K27" s="62"/>
+      <c r="L27" s="27"/>
+    </row>
+    <row r="28" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="39" t="s">
+        <v>22</v>
+      </c>
+      <c r="B28" s="11"/>
+      <c r="C28" s="82" t="s">
         <v>50</v>
       </c>
-      <c r="D21" s="21"/>
-      <c r="E21" s="21"/>
-      <c r="F21" s="21"/>
-      <c r="G21" s="21"/>
-      <c r="H21" s="21"/>
-      <c r="I21" s="21"/>
-      <c r="J21" s="21"/>
-      <c r="K21" s="73"/>
-      <c r="L21" s="70"/>
-    </row>
-    <row r="22" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="91" t="s">
-        <v>14</v>
-      </c>
-      <c r="B22" s="64"/>
-      <c r="C22" s="63" t="s">
+      <c r="D28" s="82"/>
+      <c r="E28" s="82"/>
+      <c r="F28" s="82"/>
+      <c r="G28" s="82"/>
+      <c r="H28" s="82"/>
+      <c r="I28" s="82"/>
+      <c r="J28" s="82"/>
+      <c r="K28" s="83"/>
+      <c r="L28" s="27"/>
+    </row>
+    <row r="29" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="38" t="s">
+        <v>23</v>
+      </c>
+      <c r="B29" s="11"/>
+      <c r="C29" s="80" t="s">
         <v>51</v>
       </c>
-      <c r="D22" s="63"/>
-      <c r="E22" s="63"/>
-      <c r="F22" s="63"/>
-      <c r="G22" s="63"/>
-      <c r="H22" s="63"/>
-      <c r="I22" s="63"/>
-      <c r="J22" s="63"/>
-      <c r="K22" s="75"/>
-      <c r="L22" s="70"/>
-    </row>
-    <row r="23" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="90" t="s">
-        <v>15</v>
-      </c>
-      <c r="B23" s="11"/>
-      <c r="C23" s="21" t="s">
+      <c r="D29" s="80"/>
+      <c r="E29" s="80"/>
+      <c r="F29" s="80"/>
+      <c r="G29" s="80"/>
+      <c r="H29" s="80"/>
+      <c r="I29" s="80"/>
+      <c r="J29" s="80"/>
+      <c r="K29" s="81"/>
+      <c r="L29" s="27"/>
+    </row>
+    <row r="30" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="38" t="s">
+        <v>24</v>
+      </c>
+      <c r="B30" s="11"/>
+      <c r="C30" s="80" t="s">
         <v>52</v>
       </c>
-      <c r="D23" s="21"/>
-      <c r="E23" s="21"/>
-      <c r="F23" s="21"/>
-      <c r="G23" s="21"/>
-      <c r="H23" s="21"/>
-      <c r="I23" s="21"/>
-      <c r="J23" s="21"/>
-      <c r="K23" s="73"/>
-      <c r="L23" s="70"/>
-    </row>
-    <row r="24" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="90" t="s">
-        <v>16</v>
-      </c>
-      <c r="B24" s="11"/>
-      <c r="C24" s="21" t="s">
+      <c r="D30" s="80"/>
+      <c r="E30" s="80"/>
+      <c r="F30" s="80"/>
+      <c r="G30" s="80"/>
+      <c r="H30" s="80"/>
+      <c r="I30" s="80"/>
+      <c r="J30" s="80"/>
+      <c r="K30" s="81"/>
+      <c r="L30" s="27"/>
+    </row>
+    <row r="31" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="B31" s="11"/>
+      <c r="C31" s="80" t="s">
         <v>53</v>
       </c>
-      <c r="D24" s="21"/>
-      <c r="E24" s="21"/>
-      <c r="F24" s="21"/>
-      <c r="G24" s="21"/>
-      <c r="H24" s="21"/>
-      <c r="I24" s="21"/>
-      <c r="J24" s="21"/>
-      <c r="K24" s="73"/>
-      <c r="L24" s="70"/>
-    </row>
-    <row r="25" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="92"/>
-      <c r="B25" s="58"/>
-      <c r="C25" s="59"/>
-      <c r="D25" s="59"/>
-      <c r="E25" s="59"/>
-      <c r="F25" s="59"/>
-      <c r="G25" s="59"/>
-      <c r="H25" s="59"/>
-      <c r="I25" s="59"/>
-      <c r="J25" s="59"/>
-      <c r="K25" s="76"/>
-      <c r="L25" s="70"/>
-    </row>
-    <row r="26" spans="1:13" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="93" t="s">
-        <v>21</v>
-      </c>
-      <c r="B26" s="60"/>
-      <c r="C26" s="61" t="s">
-        <v>36</v>
-      </c>
-      <c r="D26" s="62"/>
-      <c r="E26" s="62"/>
-      <c r="F26" s="62"/>
-      <c r="G26" s="62"/>
-      <c r="H26" s="62"/>
-      <c r="I26" s="62"/>
-      <c r="J26" s="62"/>
-      <c r="K26" s="74"/>
-      <c r="L26" s="70"/>
-    </row>
-    <row r="27" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="91" t="s">
-        <v>22</v>
-      </c>
-      <c r="B27" s="11"/>
-      <c r="C27" s="63" t="s">
-        <v>54</v>
-      </c>
-      <c r="D27" s="63"/>
-      <c r="E27" s="63"/>
-      <c r="F27" s="63"/>
-      <c r="G27" s="63"/>
-      <c r="H27" s="63"/>
-      <c r="I27" s="63"/>
-      <c r="J27" s="63"/>
-      <c r="K27" s="75"/>
-      <c r="L27" s="70"/>
-    </row>
-    <row r="28" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="90" t="s">
-        <v>23</v>
-      </c>
-      <c r="B28" s="11"/>
-      <c r="C28" s="21" t="s">
+      <c r="D31" s="80"/>
+      <c r="E31" s="80"/>
+      <c r="F31" s="80"/>
+      <c r="G31" s="80"/>
+      <c r="H31" s="80"/>
+      <c r="I31" s="80"/>
+      <c r="J31" s="80"/>
+      <c r="K31" s="80"/>
+      <c r="L31" s="27"/>
+    </row>
+    <row r="32" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A32" s="26"/>
+      <c r="K32" s="29"/>
+      <c r="L32" s="27"/>
+    </row>
+    <row r="33" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A33" s="41" t="s">
+        <v>25</v>
+      </c>
+      <c r="B33" s="6"/>
+      <c r="C33" s="94" t="s">
+        <v>56</v>
+      </c>
+      <c r="D33" s="94"/>
+      <c r="E33" s="94"/>
+      <c r="F33" s="94"/>
+      <c r="G33" s="94"/>
+      <c r="H33" s="94"/>
+      <c r="I33" s="94"/>
+      <c r="J33" s="94"/>
+      <c r="K33" s="95"/>
+      <c r="L33" s="27"/>
+    </row>
+    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A34" s="39" t="s">
+        <v>26</v>
+      </c>
+      <c r="B34" s="11"/>
+      <c r="C34" s="80" t="s">
+        <v>32</v>
+      </c>
+      <c r="D34" s="80"/>
+      <c r="E34" s="80"/>
+      <c r="F34" s="80"/>
+      <c r="G34" s="80"/>
+      <c r="H34" s="80"/>
+      <c r="I34" s="80"/>
+      <c r="J34" s="80"/>
+      <c r="K34" s="81"/>
+      <c r="L34" s="27"/>
+    </row>
+    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A35" s="38" t="s">
+        <v>27</v>
+      </c>
+      <c r="B35" s="11"/>
+      <c r="C35" s="80"/>
+      <c r="D35" s="80"/>
+      <c r="E35" s="80"/>
+      <c r="F35" s="80"/>
+      <c r="G35" s="80"/>
+      <c r="H35" s="80"/>
+      <c r="I35" s="80"/>
+      <c r="J35" s="80"/>
+      <c r="K35" s="81"/>
+      <c r="L35" s="27"/>
+    </row>
+    <row r="36" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A36" s="38" t="s">
+        <v>28</v>
+      </c>
+      <c r="B36" s="11"/>
+      <c r="C36" s="80"/>
+      <c r="D36" s="80"/>
+      <c r="E36" s="80"/>
+      <c r="F36" s="80"/>
+      <c r="G36" s="80"/>
+      <c r="H36" s="80"/>
+      <c r="I36" s="80"/>
+      <c r="J36" s="80"/>
+      <c r="K36" s="81"/>
+      <c r="L36" s="27"/>
+    </row>
+    <row r="37" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A37" s="38" t="s">
+        <v>29</v>
+      </c>
+      <c r="B37" s="11"/>
+      <c r="C37" s="80"/>
+      <c r="D37" s="80"/>
+      <c r="E37" s="80"/>
+      <c r="F37" s="80"/>
+      <c r="G37" s="80"/>
+      <c r="H37" s="80"/>
+      <c r="I37" s="80"/>
+      <c r="J37" s="80"/>
+      <c r="K37" s="81"/>
+      <c r="L37" s="27"/>
+    </row>
+    <row r="38" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A38" s="38" t="s">
+        <v>30</v>
+      </c>
+      <c r="B38" s="11"/>
+      <c r="C38" s="80"/>
+      <c r="D38" s="80"/>
+      <c r="E38" s="80"/>
+      <c r="F38" s="80"/>
+      <c r="G38" s="80"/>
+      <c r="H38" s="80"/>
+      <c r="I38" s="80"/>
+      <c r="J38" s="80"/>
+      <c r="K38" s="81"/>
+      <c r="L38" s="27"/>
+    </row>
+    <row r="39" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A39" s="38" t="s">
+        <v>31</v>
+      </c>
+      <c r="B39" s="11"/>
+      <c r="C39" s="80"/>
+      <c r="D39" s="80"/>
+      <c r="E39" s="80"/>
+      <c r="F39" s="80"/>
+      <c r="G39" s="80"/>
+      <c r="H39" s="80"/>
+      <c r="I39" s="80"/>
+      <c r="J39" s="80"/>
+      <c r="K39" s="81"/>
+      <c r="L39" s="27"/>
+    </row>
+    <row r="40" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A40" s="38" t="s">
+        <v>33</v>
+      </c>
+      <c r="B40" s="11"/>
+      <c r="C40" s="80" t="s">
+        <v>34</v>
+      </c>
+      <c r="D40" s="80"/>
+      <c r="E40" s="80"/>
+      <c r="F40" s="80"/>
+      <c r="G40" s="80"/>
+      <c r="H40" s="80"/>
+      <c r="I40" s="80"/>
+      <c r="J40" s="80"/>
+      <c r="K40" s="81"/>
+      <c r="L40" s="27"/>
+    </row>
+    <row r="41" spans="1:12" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A41" s="34"/>
+      <c r="B41" s="31"/>
+      <c r="C41" s="31"/>
+      <c r="D41" s="31"/>
+      <c r="E41" s="31"/>
+      <c r="F41" s="31"/>
+      <c r="G41" s="31"/>
+      <c r="H41" s="31"/>
+      <c r="I41" s="31"/>
+      <c r="J41" s="31"/>
+      <c r="K41" s="32"/>
+      <c r="L41" s="27"/>
+    </row>
+    <row r="42" spans="1:12" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A42" s="90" t="s">
         <v>55</v>
       </c>
-      <c r="D28" s="21"/>
-      <c r="E28" s="21"/>
-      <c r="F28" s="21"/>
-      <c r="G28" s="21"/>
-      <c r="H28" s="21"/>
-      <c r="I28" s="21"/>
-      <c r="J28" s="21"/>
-      <c r="K28" s="73"/>
-      <c r="L28" s="70"/>
-    </row>
-    <row r="29" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="90" t="s">
-        <v>24</v>
-      </c>
-      <c r="B29" s="11"/>
-      <c r="C29" s="21" t="s">
-        <v>56</v>
-      </c>
-      <c r="D29" s="21"/>
-      <c r="E29" s="21"/>
-      <c r="F29" s="21"/>
-      <c r="G29" s="21"/>
-      <c r="H29" s="21"/>
-      <c r="I29" s="21"/>
-      <c r="J29" s="21"/>
-      <c r="K29" s="73"/>
-      <c r="L29" s="70"/>
-    </row>
-    <row r="30" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="9" t="s">
-        <v>37</v>
-      </c>
-      <c r="B30" s="11"/>
-      <c r="C30" s="21" t="s">
-        <v>57</v>
-      </c>
-      <c r="D30" s="21"/>
-      <c r="E30" s="21"/>
-      <c r="F30" s="21"/>
-      <c r="G30" s="21"/>
-      <c r="H30" s="21"/>
-      <c r="I30" s="21"/>
-      <c r="J30" s="21"/>
-      <c r="K30" s="21"/>
-      <c r="L30" s="70"/>
-    </row>
-    <row r="31" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="69"/>
-      <c r="K31" s="72"/>
-      <c r="L31" s="70"/>
-    </row>
-    <row r="32" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="93" t="s">
-        <v>25</v>
-      </c>
-      <c r="B32" s="6"/>
-      <c r="C32" s="94" t="s">
-        <v>61</v>
-      </c>
-      <c r="D32" s="94"/>
-      <c r="E32" s="94"/>
-      <c r="F32" s="94"/>
-      <c r="G32" s="94"/>
-      <c r="H32" s="94"/>
-      <c r="I32" s="94"/>
-      <c r="J32" s="94"/>
-      <c r="K32" s="95"/>
-      <c r="L32" s="70"/>
-    </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A33" s="91" t="s">
-        <v>26</v>
-      </c>
-      <c r="B33" s="11"/>
-      <c r="C33" s="21" t="s">
-        <v>32</v>
-      </c>
-      <c r="D33" s="21"/>
-      <c r="E33" s="21"/>
-      <c r="F33" s="21"/>
-      <c r="G33" s="21"/>
-      <c r="H33" s="21"/>
-      <c r="I33" s="21"/>
-      <c r="J33" s="21"/>
-      <c r="K33" s="73"/>
-      <c r="L33" s="70"/>
-    </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A34" s="90" t="s">
-        <v>27</v>
-      </c>
-      <c r="B34" s="11"/>
-      <c r="C34" s="21"/>
-      <c r="D34" s="21"/>
-      <c r="E34" s="21"/>
-      <c r="F34" s="21"/>
-      <c r="G34" s="21"/>
-      <c r="H34" s="21"/>
-      <c r="I34" s="21"/>
-      <c r="J34" s="21"/>
-      <c r="K34" s="73"/>
-      <c r="L34" s="70"/>
-    </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A35" s="90" t="s">
-        <v>28</v>
-      </c>
-      <c r="B35" s="11"/>
-      <c r="C35" s="21"/>
-      <c r="D35" s="21"/>
-      <c r="E35" s="21"/>
-      <c r="F35" s="21"/>
-      <c r="G35" s="21"/>
-      <c r="H35" s="21"/>
-      <c r="I35" s="21"/>
-      <c r="J35" s="21"/>
-      <c r="K35" s="73"/>
-      <c r="L35" s="70"/>
-    </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A36" s="90" t="s">
-        <v>29</v>
-      </c>
-      <c r="B36" s="11"/>
-      <c r="C36" s="21"/>
-      <c r="D36" s="21"/>
-      <c r="E36" s="21"/>
-      <c r="F36" s="21"/>
-      <c r="G36" s="21"/>
-      <c r="H36" s="21"/>
-      <c r="I36" s="21"/>
-      <c r="J36" s="21"/>
-      <c r="K36" s="73"/>
-      <c r="L36" s="70"/>
-    </row>
-    <row r="37" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A37" s="90" t="s">
-        <v>30</v>
-      </c>
-      <c r="B37" s="11"/>
-      <c r="C37" s="21"/>
-      <c r="D37" s="21"/>
-      <c r="E37" s="21"/>
-      <c r="F37" s="21"/>
-      <c r="G37" s="21"/>
-      <c r="H37" s="21"/>
-      <c r="I37" s="21"/>
-      <c r="J37" s="21"/>
-      <c r="K37" s="73"/>
-      <c r="L37" s="70"/>
-    </row>
-    <row r="38" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A38" s="90" t="s">
-        <v>31</v>
-      </c>
-      <c r="B38" s="11"/>
-      <c r="C38" s="21"/>
-      <c r="D38" s="21"/>
-      <c r="E38" s="21"/>
-      <c r="F38" s="21"/>
-      <c r="G38" s="21"/>
-      <c r="H38" s="21"/>
-      <c r="I38" s="21"/>
-      <c r="J38" s="21"/>
-      <c r="K38" s="73"/>
-      <c r="L38" s="70"/>
-    </row>
-    <row r="39" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A39" s="90" t="s">
-        <v>33</v>
-      </c>
-      <c r="B39" s="11"/>
-      <c r="C39" s="21" t="s">
-        <v>34</v>
-      </c>
-      <c r="D39" s="21"/>
-      <c r="E39" s="21"/>
-      <c r="F39" s="21"/>
-      <c r="G39" s="21"/>
-      <c r="H39" s="21"/>
-      <c r="I39" s="21"/>
-      <c r="J39" s="21"/>
-      <c r="K39" s="73"/>
-      <c r="L39" s="70"/>
-    </row>
-    <row r="40" spans="1:12" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A40" s="86"/>
-      <c r="B40" s="79"/>
-      <c r="C40" s="79"/>
-      <c r="D40" s="79"/>
-      <c r="E40" s="79"/>
-      <c r="F40" s="79"/>
-      <c r="G40" s="79"/>
-      <c r="H40" s="79"/>
-      <c r="I40" s="79"/>
-      <c r="J40" s="79"/>
-      <c r="K40" s="80"/>
-      <c r="L40" s="70"/>
-    </row>
-    <row r="41" spans="1:12" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="83" t="s">
-        <v>60</v>
-      </c>
-      <c r="B41" s="84"/>
-      <c r="C41" s="84"/>
-      <c r="D41" s="84"/>
-      <c r="E41" s="84"/>
-      <c r="F41" s="84"/>
-      <c r="G41" s="84"/>
-      <c r="H41" s="84"/>
-      <c r="I41" s="84"/>
-      <c r="J41" s="84"/>
-      <c r="K41" s="84"/>
-      <c r="L41" s="70"/>
-    </row>
-    <row r="42" spans="1:12" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A42" s="85"/>
-      <c r="B42" s="82"/>
-      <c r="C42" s="82"/>
-      <c r="D42" s="82"/>
-      <c r="E42" s="82"/>
-      <c r="F42" s="82"/>
-      <c r="G42" s="82"/>
-      <c r="H42" s="82"/>
-      <c r="I42" s="82"/>
-      <c r="J42" s="82"/>
-      <c r="K42" s="82"/>
-      <c r="L42" s="81"/>
-    </row>
-    <row r="43" spans="1:12" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+      <c r="B42" s="91"/>
+      <c r="C42" s="91"/>
+      <c r="D42" s="91"/>
+      <c r="E42" s="91"/>
+      <c r="F42" s="91"/>
+      <c r="G42" s="91"/>
+      <c r="H42" s="91"/>
+      <c r="I42" s="91"/>
+      <c r="J42" s="91"/>
+      <c r="K42" s="91"/>
+      <c r="L42" s="27"/>
+    </row>
+    <row r="43" spans="1:12" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A43" s="92"/>
+      <c r="B43" s="93"/>
+      <c r="C43" s="93"/>
+      <c r="D43" s="93"/>
+      <c r="E43" s="93"/>
+      <c r="F43" s="93"/>
+      <c r="G43" s="93"/>
+      <c r="H43" s="93"/>
+      <c r="I43" s="93"/>
+      <c r="J43" s="93"/>
+      <c r="K43" s="93"/>
+      <c r="L43" s="33"/>
+    </row>
+    <row r="44" spans="1:12" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
   </sheetData>
-  <mergeCells count="24">
-    <mergeCell ref="C15:K15"/>
+  <mergeCells count="25">
+    <mergeCell ref="C12:K13"/>
+    <mergeCell ref="C40:K40"/>
+    <mergeCell ref="A42:K43"/>
+    <mergeCell ref="C28:K28"/>
+    <mergeCell ref="C29:K29"/>
+    <mergeCell ref="C30:K30"/>
+    <mergeCell ref="C31:K31"/>
+    <mergeCell ref="C33:K33"/>
+    <mergeCell ref="C34:K39"/>
     <mergeCell ref="C16:K16"/>
-    <mergeCell ref="C18:K18"/>
-    <mergeCell ref="C26:K26"/>
+    <mergeCell ref="C17:K17"/>
+    <mergeCell ref="C19:K19"/>
+    <mergeCell ref="C27:K27"/>
     <mergeCell ref="A1:K4"/>
     <mergeCell ref="C7:K8"/>
-    <mergeCell ref="C11:K12"/>
-    <mergeCell ref="C19:K19"/>
+    <mergeCell ref="C11:K11"/>
     <mergeCell ref="C20:K20"/>
     <mergeCell ref="C21:K21"/>
     <mergeCell ref="C22:K22"/>
     <mergeCell ref="C23:K23"/>
     <mergeCell ref="C24:K24"/>
+    <mergeCell ref="C25:K25"/>
     <mergeCell ref="C6:K6"/>
-    <mergeCell ref="C13:K13"/>
     <mergeCell ref="C14:K14"/>
-    <mergeCell ref="C39:K39"/>
-    <mergeCell ref="A41:K42"/>
-    <mergeCell ref="C27:K27"/>
-    <mergeCell ref="C28:K28"/>
-    <mergeCell ref="C29:K29"/>
-    <mergeCell ref="C30:K30"/>
-    <mergeCell ref="C32:K32"/>
-    <mergeCell ref="C33:K38"/>
+    <mergeCell ref="C15:K15"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
Update documentation and descriptions to say Line-to-line nominal voltage instead of just nominal voltage
</commit_message>
<xml_diff>
--- a/Source/Documentation/Device Definitions Examples & Templates/openXDA Configuration Template - DFR.xlsx
+++ b/Source/Documentation/Device Definitions Examples & Templates/openXDA Configuration Template - DFR.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17329"/>
-  <workbookPr defaultThemeVersion="164011"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19001"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\openXDA\Source\Documentation\Device Definitions Examples &amp; Templates\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sjenks\Documents\Projects\GitHub\openXDA\Source\Documentation\Device Definitions Examples &amp; Templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -188,8 +188,56 @@
     </r>
   </si>
   <si>
+    <t>Accurate line length, specified in miles by default: numeric decimal value</t>
+  </si>
+  <si>
+    <t>stationID at the other end of the line if a reporting device is located there: up to 50 char</t>
+  </si>
+  <si>
+    <t>stationName at the other end of the line if a reporting device is located there: up to 200 char</t>
+  </si>
+  <si>
+    <t>Positive sequence resistance: nummeric decimal value</t>
+  </si>
+  <si>
+    <t>Zero sequence resistance: nummeric decimal value</t>
+  </si>
+  <si>
+    <t>Positive sequence reactance: nummeric decimal value</t>
+  </si>
+  <si>
+    <t>Zero sequence reactance: nummeric decimal value</t>
+  </si>
+  <si>
+    <t>As a general rule, the device id is the name of the folder where the data is stored for that device. DFR data should be in COMTRADE or native E-Max format.</t>
+  </si>
+  <si>
+    <t>If a device is monitoring more than one line, please copy the section outlined in blue and paste it below, then fill in the appropriate information.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Channel definitions are only required for COMTRADE input files. </t>
+  </si>
+  <si>
+    <t>Specific information about the reporting device; DFR etc. Up to 200 characters each for make and model fields.</t>
+  </si>
+  <si>
+    <t>Unique ID for the location of the device: Up to 50 characters.</t>
+  </si>
+  <si>
+    <t>Human readable name for the location: Up to 200 characters.</t>
+  </si>
+  <si>
+    <t>Human readable name for the reporting device; DFR etc. Up to 200 characters.</t>
+  </si>
+  <si>
+    <t>Human readable name for the line or location: Up to 200 characters.</t>
+  </si>
+  <si>
+    <t>This template is intended for use in configuring an openXDA database for data from substation devices such as digital fault recorders; one device per template. A separate template is available for PQ monitors and relays. Each device must be defined by specifying the information described below. Please enter a value for each parameter. "ID" fields are limited to 50 characters, other non-numeric fields can contain up to 200 characters.</t>
+  </si>
+  <si>
     <r>
-      <t>Nominal voltage in</t>
+      <t>Line-to-line Nominal voltage in</t>
     </r>
     <r>
       <rPr>
@@ -212,54 +260,6 @@
       </rPr>
       <t>: numeric decimal value</t>
     </r>
-  </si>
-  <si>
-    <t>Accurate line length, specified in miles by default: numeric decimal value</t>
-  </si>
-  <si>
-    <t>stationID at the other end of the line if a reporting device is located there: up to 50 char</t>
-  </si>
-  <si>
-    <t>stationName at the other end of the line if a reporting device is located there: up to 200 char</t>
-  </si>
-  <si>
-    <t>Positive sequence resistance: nummeric decimal value</t>
-  </si>
-  <si>
-    <t>Zero sequence resistance: nummeric decimal value</t>
-  </si>
-  <si>
-    <t>Positive sequence reactance: nummeric decimal value</t>
-  </si>
-  <si>
-    <t>Zero sequence reactance: nummeric decimal value</t>
-  </si>
-  <si>
-    <t>As a general rule, the device id is the name of the folder where the data is stored for that device. DFR data should be in COMTRADE or native E-Max format.</t>
-  </si>
-  <si>
-    <t>If a device is monitoring more than one line, please copy the section outlined in blue and paste it below, then fill in the appropriate information.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Channel definitions are only required for COMTRADE input files. </t>
-  </si>
-  <si>
-    <t>Specific information about the reporting device; DFR etc. Up to 200 characters each for make and model fields.</t>
-  </si>
-  <si>
-    <t>Unique ID for the location of the device: Up to 50 characters.</t>
-  </si>
-  <si>
-    <t>Human readable name for the location: Up to 200 characters.</t>
-  </si>
-  <si>
-    <t>Human readable name for the reporting device; DFR etc. Up to 200 characters.</t>
-  </si>
-  <si>
-    <t>Human readable name for the line or location: Up to 200 characters.</t>
-  </si>
-  <si>
-    <t>This template is intended for use in configuring an openXDA database for data from substation devices such as digital fault recorders; one device per template. A separate template is available for PQ monitors and relays. Each device must be defined by specifying the information described below. Please enter a value for each parameter. "ID" fields are limited to 50 characters, other non-numeric fields can contain up to 200 characters.</t>
   </si>
 </sst>
 </file>
@@ -1113,6 +1113,48 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="38" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="46" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="47" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="48" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="44" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="40" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -1182,36 +1224,12 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="38" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="38" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="40" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
@@ -1229,24 +1247,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="46" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="47" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="48" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="44" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1681,8 +1681,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M44"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:K4"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="C22" sqref="C22:K22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1693,58 +1693,58 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="63" t="s">
-        <v>62</v>
-      </c>
-      <c r="B1" s="64"/>
-      <c r="C1" s="64"/>
-      <c r="D1" s="64"/>
-      <c r="E1" s="64"/>
-      <c r="F1" s="64"/>
-      <c r="G1" s="64"/>
-      <c r="H1" s="64"/>
-      <c r="I1" s="64"/>
-      <c r="J1" s="64"/>
-      <c r="K1" s="65"/>
+      <c r="A1" s="77" t="s">
+        <v>61</v>
+      </c>
+      <c r="B1" s="78"/>
+      <c r="C1" s="78"/>
+      <c r="D1" s="78"/>
+      <c r="E1" s="78"/>
+      <c r="F1" s="78"/>
+      <c r="G1" s="78"/>
+      <c r="H1" s="78"/>
+      <c r="I1" s="78"/>
+      <c r="J1" s="78"/>
+      <c r="K1" s="79"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A2" s="66"/>
-      <c r="B2" s="67"/>
-      <c r="C2" s="67"/>
-      <c r="D2" s="67"/>
-      <c r="E2" s="67"/>
-      <c r="F2" s="67"/>
-      <c r="G2" s="67"/>
-      <c r="H2" s="67"/>
-      <c r="I2" s="67"/>
-      <c r="J2" s="67"/>
-      <c r="K2" s="68"/>
+      <c r="A2" s="80"/>
+      <c r="B2" s="81"/>
+      <c r="C2" s="81"/>
+      <c r="D2" s="81"/>
+      <c r="E2" s="81"/>
+      <c r="F2" s="81"/>
+      <c r="G2" s="81"/>
+      <c r="H2" s="81"/>
+      <c r="I2" s="81"/>
+      <c r="J2" s="81"/>
+      <c r="K2" s="82"/>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A3" s="66"/>
-      <c r="B3" s="67"/>
-      <c r="C3" s="67"/>
-      <c r="D3" s="67"/>
-      <c r="E3" s="67"/>
-      <c r="F3" s="67"/>
-      <c r="G3" s="67"/>
-      <c r="H3" s="67"/>
-      <c r="I3" s="67"/>
-      <c r="J3" s="67"/>
-      <c r="K3" s="68"/>
+      <c r="A3" s="80"/>
+      <c r="B3" s="81"/>
+      <c r="C3" s="81"/>
+      <c r="D3" s="81"/>
+      <c r="E3" s="81"/>
+      <c r="F3" s="81"/>
+      <c r="G3" s="81"/>
+      <c r="H3" s="81"/>
+      <c r="I3" s="81"/>
+      <c r="J3" s="81"/>
+      <c r="K3" s="82"/>
     </row>
     <row r="4" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="69"/>
-      <c r="B4" s="70"/>
-      <c r="C4" s="70"/>
-      <c r="D4" s="70"/>
-      <c r="E4" s="70"/>
-      <c r="F4" s="70"/>
-      <c r="G4" s="70"/>
-      <c r="H4" s="70"/>
-      <c r="I4" s="70"/>
-      <c r="J4" s="70"/>
-      <c r="K4" s="71"/>
+      <c r="A4" s="83"/>
+      <c r="B4" s="84"/>
+      <c r="C4" s="84"/>
+      <c r="D4" s="84"/>
+      <c r="E4" s="84"/>
+      <c r="F4" s="84"/>
+      <c r="G4" s="84"/>
+      <c r="H4" s="84"/>
+      <c r="I4" s="84"/>
+      <c r="J4" s="84"/>
+      <c r="K4" s="85"/>
     </row>
     <row r="5" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="6" spans="1:11" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -1754,47 +1754,47 @@
       <c r="B6" s="10" t="s">
         <v>40</v>
       </c>
-      <c r="C6" s="84" t="s">
+      <c r="C6" s="90" t="s">
         <v>41</v>
       </c>
-      <c r="D6" s="85"/>
-      <c r="E6" s="85"/>
-      <c r="F6" s="85"/>
-      <c r="G6" s="85"/>
-      <c r="H6" s="85"/>
-      <c r="I6" s="85"/>
-      <c r="J6" s="85"/>
-      <c r="K6" s="86"/>
+      <c r="D6" s="91"/>
+      <c r="E6" s="91"/>
+      <c r="F6" s="91"/>
+      <c r="G6" s="91"/>
+      <c r="H6" s="91"/>
+      <c r="I6" s="91"/>
+      <c r="J6" s="91"/>
+      <c r="K6" s="92"/>
     </row>
     <row r="7" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
         <v>11</v>
       </c>
       <c r="B7" s="11"/>
-      <c r="C7" s="72" t="s">
-        <v>54</v>
-      </c>
-      <c r="D7" s="72"/>
-      <c r="E7" s="72"/>
-      <c r="F7" s="72"/>
-      <c r="G7" s="72"/>
-      <c r="H7" s="72"/>
-      <c r="I7" s="72"/>
-      <c r="J7" s="72"/>
-      <c r="K7" s="72"/>
+      <c r="C7" s="86" t="s">
+        <v>53</v>
+      </c>
+      <c r="D7" s="86"/>
+      <c r="E7" s="86"/>
+      <c r="F7" s="86"/>
+      <c r="G7" s="86"/>
+      <c r="H7" s="86"/>
+      <c r="I7" s="86"/>
+      <c r="J7" s="86"/>
+      <c r="K7" s="86"/>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="8"/>
       <c r="B8" s="8"/>
-      <c r="C8" s="73"/>
-      <c r="D8" s="73"/>
-      <c r="E8" s="73"/>
-      <c r="F8" s="73"/>
-      <c r="G8" s="73"/>
-      <c r="H8" s="73"/>
-      <c r="I8" s="73"/>
-      <c r="J8" s="73"/>
-      <c r="K8" s="73"/>
+      <c r="C8" s="87"/>
+      <c r="D8" s="87"/>
+      <c r="E8" s="87"/>
+      <c r="F8" s="87"/>
+      <c r="G8" s="87"/>
+      <c r="H8" s="87"/>
+      <c r="I8" s="87"/>
+      <c r="J8" s="87"/>
+      <c r="K8" s="87"/>
     </row>
     <row r="9" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="10" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1817,117 +1817,117 @@
         <v>12</v>
       </c>
       <c r="B11" s="14"/>
-      <c r="C11" s="74" t="s">
-        <v>60</v>
-      </c>
-      <c r="D11" s="74"/>
-      <c r="E11" s="74"/>
-      <c r="F11" s="74"/>
-      <c r="G11" s="74"/>
-      <c r="H11" s="74"/>
-      <c r="I11" s="74"/>
-      <c r="J11" s="74"/>
-      <c r="K11" s="75"/>
+      <c r="C11" s="51" t="s">
+        <v>59</v>
+      </c>
+      <c r="D11" s="51"/>
+      <c r="E11" s="51"/>
+      <c r="F11" s="51"/>
+      <c r="G11" s="51"/>
+      <c r="H11" s="51"/>
+      <c r="I11" s="51"/>
+      <c r="J11" s="51"/>
+      <c r="K11" s="52"/>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="13" t="s">
         <v>17</v>
       </c>
       <c r="B12" s="14"/>
-      <c r="C12" s="74" t="s">
-        <v>57</v>
-      </c>
-      <c r="D12" s="74"/>
-      <c r="E12" s="74"/>
-      <c r="F12" s="74"/>
-      <c r="G12" s="74"/>
-      <c r="H12" s="74"/>
-      <c r="I12" s="74"/>
-      <c r="J12" s="74"/>
-      <c r="K12" s="75"/>
+      <c r="C12" s="51" t="s">
+        <v>56</v>
+      </c>
+      <c r="D12" s="51"/>
+      <c r="E12" s="51"/>
+      <c r="F12" s="51"/>
+      <c r="G12" s="51"/>
+      <c r="H12" s="51"/>
+      <c r="I12" s="51"/>
+      <c r="J12" s="51"/>
+      <c r="K12" s="52"/>
     </row>
     <row r="13" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="15" t="s">
         <v>18</v>
       </c>
       <c r="B13" s="16"/>
-      <c r="C13" s="76"/>
-      <c r="D13" s="76"/>
-      <c r="E13" s="76"/>
-      <c r="F13" s="76"/>
-      <c r="G13" s="76"/>
-      <c r="H13" s="76"/>
-      <c r="I13" s="76"/>
-      <c r="J13" s="76"/>
-      <c r="K13" s="77"/>
+      <c r="C13" s="53"/>
+      <c r="D13" s="53"/>
+      <c r="E13" s="53"/>
+      <c r="F13" s="53"/>
+      <c r="G13" s="53"/>
+      <c r="H13" s="53"/>
+      <c r="I13" s="53"/>
+      <c r="J13" s="53"/>
+      <c r="K13" s="54"/>
     </row>
     <row r="14" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="13" t="s">
         <v>19</v>
       </c>
       <c r="B14" s="14"/>
-      <c r="C14" s="87" t="s">
-        <v>58</v>
-      </c>
-      <c r="D14" s="88"/>
-      <c r="E14" s="88"/>
-      <c r="F14" s="88"/>
-      <c r="G14" s="88"/>
-      <c r="H14" s="88"/>
-      <c r="I14" s="88"/>
-      <c r="J14" s="88"/>
-      <c r="K14" s="89"/>
+      <c r="C14" s="93" t="s">
+        <v>57</v>
+      </c>
+      <c r="D14" s="94"/>
+      <c r="E14" s="94"/>
+      <c r="F14" s="94"/>
+      <c r="G14" s="94"/>
+      <c r="H14" s="94"/>
+      <c r="I14" s="94"/>
+      <c r="J14" s="94"/>
+      <c r="K14" s="95"/>
     </row>
     <row r="15" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="17" t="s">
         <v>20</v>
       </c>
       <c r="B15" s="11"/>
-      <c r="C15" s="51" t="s">
-        <v>59</v>
-      </c>
-      <c r="D15" s="52"/>
-      <c r="E15" s="52"/>
-      <c r="F15" s="52"/>
-      <c r="G15" s="52"/>
-      <c r="H15" s="52"/>
-      <c r="I15" s="52"/>
-      <c r="J15" s="52"/>
-      <c r="K15" s="53"/>
+      <c r="C15" s="65" t="s">
+        <v>58</v>
+      </c>
+      <c r="D15" s="66"/>
+      <c r="E15" s="66"/>
+      <c r="F15" s="66"/>
+      <c r="G15" s="66"/>
+      <c r="H15" s="66"/>
+      <c r="I15" s="66"/>
+      <c r="J15" s="66"/>
+      <c r="K15" s="67"/>
     </row>
     <row r="16" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="18" t="s">
         <v>38</v>
       </c>
       <c r="B16" s="11"/>
-      <c r="C16" s="51" t="s">
+      <c r="C16" s="65" t="s">
         <v>42</v>
       </c>
-      <c r="D16" s="52"/>
-      <c r="E16" s="52"/>
-      <c r="F16" s="52"/>
-      <c r="G16" s="52"/>
-      <c r="H16" s="52"/>
-      <c r="I16" s="52"/>
-      <c r="J16" s="52"/>
-      <c r="K16" s="53"/>
+      <c r="D16" s="66"/>
+      <c r="E16" s="66"/>
+      <c r="F16" s="66"/>
+      <c r="G16" s="66"/>
+      <c r="H16" s="66"/>
+      <c r="I16" s="66"/>
+      <c r="J16" s="66"/>
+      <c r="K16" s="67"/>
     </row>
     <row r="17" spans="1:13" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="19" t="s">
         <v>39</v>
       </c>
       <c r="B17" s="16"/>
-      <c r="C17" s="54" t="s">
+      <c r="C17" s="68" t="s">
         <v>42</v>
       </c>
-      <c r="D17" s="55"/>
-      <c r="E17" s="55"/>
-      <c r="F17" s="55"/>
-      <c r="G17" s="55"/>
-      <c r="H17" s="55"/>
-      <c r="I17" s="55"/>
-      <c r="J17" s="55"/>
-      <c r="K17" s="56"/>
+      <c r="D17" s="69"/>
+      <c r="E17" s="69"/>
+      <c r="F17" s="69"/>
+      <c r="G17" s="69"/>
+      <c r="H17" s="69"/>
+      <c r="I17" s="69"/>
+      <c r="J17" s="69"/>
+      <c r="K17" s="70"/>
     </row>
     <row r="18" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="35"/>
@@ -1938,17 +1938,17 @@
         <v>43</v>
       </c>
       <c r="B19" s="24"/>
-      <c r="C19" s="57" t="s">
+      <c r="C19" s="71" t="s">
         <v>44</v>
       </c>
-      <c r="D19" s="58"/>
-      <c r="E19" s="58"/>
-      <c r="F19" s="58"/>
-      <c r="G19" s="58"/>
-      <c r="H19" s="58"/>
-      <c r="I19" s="58"/>
-      <c r="J19" s="58"/>
-      <c r="K19" s="59"/>
+      <c r="D19" s="72"/>
+      <c r="E19" s="72"/>
+      <c r="F19" s="72"/>
+      <c r="G19" s="72"/>
+      <c r="H19" s="72"/>
+      <c r="I19" s="72"/>
+      <c r="J19" s="72"/>
+      <c r="K19" s="73"/>
       <c r="L19" s="28"/>
       <c r="M19" s="20"/>
     </row>
@@ -1957,17 +1957,17 @@
         <v>10</v>
       </c>
       <c r="B20" s="11"/>
-      <c r="C20" s="78" t="s">
+      <c r="C20" s="88" t="s">
         <v>45</v>
       </c>
-      <c r="D20" s="78"/>
-      <c r="E20" s="78"/>
-      <c r="F20" s="78"/>
-      <c r="G20" s="78"/>
-      <c r="H20" s="78"/>
-      <c r="I20" s="78"/>
-      <c r="J20" s="78"/>
-      <c r="K20" s="79"/>
+      <c r="D20" s="88"/>
+      <c r="E20" s="88"/>
+      <c r="F20" s="88"/>
+      <c r="G20" s="88"/>
+      <c r="H20" s="88"/>
+      <c r="I20" s="88"/>
+      <c r="J20" s="88"/>
+      <c r="K20" s="89"/>
       <c r="L20" s="27"/>
       <c r="M20" s="20"/>
     </row>
@@ -1976,17 +1976,17 @@
         <v>12</v>
       </c>
       <c r="B21" s="11"/>
-      <c r="C21" s="80" t="s">
-        <v>61</v>
-      </c>
-      <c r="D21" s="80"/>
-      <c r="E21" s="80"/>
-      <c r="F21" s="80"/>
-      <c r="G21" s="80"/>
-      <c r="H21" s="80"/>
-      <c r="I21" s="80"/>
-      <c r="J21" s="80"/>
-      <c r="K21" s="81"/>
+      <c r="C21" s="55" t="s">
+        <v>60</v>
+      </c>
+      <c r="D21" s="55"/>
+      <c r="E21" s="55"/>
+      <c r="F21" s="55"/>
+      <c r="G21" s="55"/>
+      <c r="H21" s="55"/>
+      <c r="I21" s="55"/>
+      <c r="J21" s="55"/>
+      <c r="K21" s="56"/>
       <c r="L21" s="27"/>
       <c r="M21" s="20"/>
     </row>
@@ -1995,17 +1995,17 @@
         <v>13</v>
       </c>
       <c r="B22" s="11"/>
-      <c r="C22" s="80" t="s">
-        <v>46</v>
-      </c>
-      <c r="D22" s="80"/>
-      <c r="E22" s="80"/>
-      <c r="F22" s="80"/>
-      <c r="G22" s="80"/>
-      <c r="H22" s="80"/>
-      <c r="I22" s="80"/>
-      <c r="J22" s="80"/>
-      <c r="K22" s="81"/>
+      <c r="C22" s="55" t="s">
+        <v>62</v>
+      </c>
+      <c r="D22" s="55"/>
+      <c r="E22" s="55"/>
+      <c r="F22" s="55"/>
+      <c r="G22" s="55"/>
+      <c r="H22" s="55"/>
+      <c r="I22" s="55"/>
+      <c r="J22" s="55"/>
+      <c r="K22" s="56"/>
       <c r="L22" s="27"/>
     </row>
     <row r="23" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -2013,17 +2013,17 @@
         <v>14</v>
       </c>
       <c r="B23" s="23"/>
-      <c r="C23" s="82" t="s">
-        <v>47</v>
-      </c>
-      <c r="D23" s="82"/>
-      <c r="E23" s="82"/>
-      <c r="F23" s="82"/>
-      <c r="G23" s="82"/>
-      <c r="H23" s="82"/>
-      <c r="I23" s="82"/>
-      <c r="J23" s="82"/>
-      <c r="K23" s="83"/>
+      <c r="C23" s="61" t="s">
+        <v>46</v>
+      </c>
+      <c r="D23" s="61"/>
+      <c r="E23" s="61"/>
+      <c r="F23" s="61"/>
+      <c r="G23" s="61"/>
+      <c r="H23" s="61"/>
+      <c r="I23" s="61"/>
+      <c r="J23" s="61"/>
+      <c r="K23" s="62"/>
       <c r="L23" s="27"/>
     </row>
     <row r="24" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -2031,17 +2031,17 @@
         <v>15</v>
       </c>
       <c r="B24" s="11"/>
-      <c r="C24" s="80" t="s">
-        <v>48</v>
-      </c>
-      <c r="D24" s="80"/>
-      <c r="E24" s="80"/>
-      <c r="F24" s="80"/>
-      <c r="G24" s="80"/>
-      <c r="H24" s="80"/>
-      <c r="I24" s="80"/>
-      <c r="J24" s="80"/>
-      <c r="K24" s="81"/>
+      <c r="C24" s="55" t="s">
+        <v>47</v>
+      </c>
+      <c r="D24" s="55"/>
+      <c r="E24" s="55"/>
+      <c r="F24" s="55"/>
+      <c r="G24" s="55"/>
+      <c r="H24" s="55"/>
+      <c r="I24" s="55"/>
+      <c r="J24" s="55"/>
+      <c r="K24" s="56"/>
       <c r="L24" s="27"/>
     </row>
     <row r="25" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -2049,17 +2049,17 @@
         <v>16</v>
       </c>
       <c r="B25" s="11"/>
-      <c r="C25" s="80" t="s">
-        <v>49</v>
-      </c>
-      <c r="D25" s="80"/>
-      <c r="E25" s="80"/>
-      <c r="F25" s="80"/>
-      <c r="G25" s="80"/>
-      <c r="H25" s="80"/>
-      <c r="I25" s="80"/>
-      <c r="J25" s="80"/>
-      <c r="K25" s="81"/>
+      <c r="C25" s="55" t="s">
+        <v>48</v>
+      </c>
+      <c r="D25" s="55"/>
+      <c r="E25" s="55"/>
+      <c r="F25" s="55"/>
+      <c r="G25" s="55"/>
+      <c r="H25" s="55"/>
+      <c r="I25" s="55"/>
+      <c r="J25" s="55"/>
+      <c r="K25" s="56"/>
       <c r="L25" s="27"/>
     </row>
     <row r="26" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2081,17 +2081,17 @@
         <v>21</v>
       </c>
       <c r="B27" s="22"/>
-      <c r="C27" s="60" t="s">
+      <c r="C27" s="74" t="s">
         <v>36</v>
       </c>
-      <c r="D27" s="61"/>
-      <c r="E27" s="61"/>
-      <c r="F27" s="61"/>
-      <c r="G27" s="61"/>
-      <c r="H27" s="61"/>
-      <c r="I27" s="61"/>
-      <c r="J27" s="61"/>
-      <c r="K27" s="62"/>
+      <c r="D27" s="75"/>
+      <c r="E27" s="75"/>
+      <c r="F27" s="75"/>
+      <c r="G27" s="75"/>
+      <c r="H27" s="75"/>
+      <c r="I27" s="75"/>
+      <c r="J27" s="75"/>
+      <c r="K27" s="76"/>
       <c r="L27" s="27"/>
     </row>
     <row r="28" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -2099,17 +2099,17 @@
         <v>22</v>
       </c>
       <c r="B28" s="11"/>
-      <c r="C28" s="82" t="s">
-        <v>50</v>
-      </c>
-      <c r="D28" s="82"/>
-      <c r="E28" s="82"/>
-      <c r="F28" s="82"/>
-      <c r="G28" s="82"/>
-      <c r="H28" s="82"/>
-      <c r="I28" s="82"/>
-      <c r="J28" s="82"/>
-      <c r="K28" s="83"/>
+      <c r="C28" s="61" t="s">
+        <v>49</v>
+      </c>
+      <c r="D28" s="61"/>
+      <c r="E28" s="61"/>
+      <c r="F28" s="61"/>
+      <c r="G28" s="61"/>
+      <c r="H28" s="61"/>
+      <c r="I28" s="61"/>
+      <c r="J28" s="61"/>
+      <c r="K28" s="62"/>
       <c r="L28" s="27"/>
     </row>
     <row r="29" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -2117,17 +2117,17 @@
         <v>23</v>
       </c>
       <c r="B29" s="11"/>
-      <c r="C29" s="80" t="s">
-        <v>51</v>
-      </c>
-      <c r="D29" s="80"/>
-      <c r="E29" s="80"/>
-      <c r="F29" s="80"/>
-      <c r="G29" s="80"/>
-      <c r="H29" s="80"/>
-      <c r="I29" s="80"/>
-      <c r="J29" s="80"/>
-      <c r="K29" s="81"/>
+      <c r="C29" s="55" t="s">
+        <v>50</v>
+      </c>
+      <c r="D29" s="55"/>
+      <c r="E29" s="55"/>
+      <c r="F29" s="55"/>
+      <c r="G29" s="55"/>
+      <c r="H29" s="55"/>
+      <c r="I29" s="55"/>
+      <c r="J29" s="55"/>
+      <c r="K29" s="56"/>
       <c r="L29" s="27"/>
     </row>
     <row r="30" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -2135,17 +2135,17 @@
         <v>24</v>
       </c>
       <c r="B30" s="11"/>
-      <c r="C30" s="80" t="s">
-        <v>52</v>
-      </c>
-      <c r="D30" s="80"/>
-      <c r="E30" s="80"/>
-      <c r="F30" s="80"/>
-      <c r="G30" s="80"/>
-      <c r="H30" s="80"/>
-      <c r="I30" s="80"/>
-      <c r="J30" s="80"/>
-      <c r="K30" s="81"/>
+      <c r="C30" s="55" t="s">
+        <v>51</v>
+      </c>
+      <c r="D30" s="55"/>
+      <c r="E30" s="55"/>
+      <c r="F30" s="55"/>
+      <c r="G30" s="55"/>
+      <c r="H30" s="55"/>
+      <c r="I30" s="55"/>
+      <c r="J30" s="55"/>
+      <c r="K30" s="56"/>
       <c r="L30" s="27"/>
     </row>
     <row r="31" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -2153,17 +2153,17 @@
         <v>37</v>
       </c>
       <c r="B31" s="11"/>
-      <c r="C31" s="80" t="s">
-        <v>53</v>
-      </c>
-      <c r="D31" s="80"/>
-      <c r="E31" s="80"/>
-      <c r="F31" s="80"/>
-      <c r="G31" s="80"/>
-      <c r="H31" s="80"/>
-      <c r="I31" s="80"/>
-      <c r="J31" s="80"/>
-      <c r="K31" s="80"/>
+      <c r="C31" s="55" t="s">
+        <v>52</v>
+      </c>
+      <c r="D31" s="55"/>
+      <c r="E31" s="55"/>
+      <c r="F31" s="55"/>
+      <c r="G31" s="55"/>
+      <c r="H31" s="55"/>
+      <c r="I31" s="55"/>
+      <c r="J31" s="55"/>
+      <c r="K31" s="55"/>
       <c r="L31" s="27"/>
     </row>
     <row r="32" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2176,17 +2176,17 @@
         <v>25</v>
       </c>
       <c r="B33" s="6"/>
-      <c r="C33" s="94" t="s">
-        <v>56</v>
-      </c>
-      <c r="D33" s="94"/>
-      <c r="E33" s="94"/>
-      <c r="F33" s="94"/>
-      <c r="G33" s="94"/>
-      <c r="H33" s="94"/>
-      <c r="I33" s="94"/>
-      <c r="J33" s="94"/>
-      <c r="K33" s="95"/>
+      <c r="C33" s="63" t="s">
+        <v>55</v>
+      </c>
+      <c r="D33" s="63"/>
+      <c r="E33" s="63"/>
+      <c r="F33" s="63"/>
+      <c r="G33" s="63"/>
+      <c r="H33" s="63"/>
+      <c r="I33" s="63"/>
+      <c r="J33" s="63"/>
+      <c r="K33" s="64"/>
       <c r="L33" s="27"/>
     </row>
     <row r="34" spans="1:12" x14ac:dyDescent="0.25">
@@ -2194,17 +2194,17 @@
         <v>26</v>
       </c>
       <c r="B34" s="11"/>
-      <c r="C34" s="80" t="s">
+      <c r="C34" s="55" t="s">
         <v>32</v>
       </c>
-      <c r="D34" s="80"/>
-      <c r="E34" s="80"/>
-      <c r="F34" s="80"/>
-      <c r="G34" s="80"/>
-      <c r="H34" s="80"/>
-      <c r="I34" s="80"/>
-      <c r="J34" s="80"/>
-      <c r="K34" s="81"/>
+      <c r="D34" s="55"/>
+      <c r="E34" s="55"/>
+      <c r="F34" s="55"/>
+      <c r="G34" s="55"/>
+      <c r="H34" s="55"/>
+      <c r="I34" s="55"/>
+      <c r="J34" s="55"/>
+      <c r="K34" s="56"/>
       <c r="L34" s="27"/>
     </row>
     <row r="35" spans="1:12" x14ac:dyDescent="0.25">
@@ -2212,15 +2212,15 @@
         <v>27</v>
       </c>
       <c r="B35" s="11"/>
-      <c r="C35" s="80"/>
-      <c r="D35" s="80"/>
-      <c r="E35" s="80"/>
-      <c r="F35" s="80"/>
-      <c r="G35" s="80"/>
-      <c r="H35" s="80"/>
-      <c r="I35" s="80"/>
-      <c r="J35" s="80"/>
-      <c r="K35" s="81"/>
+      <c r="C35" s="55"/>
+      <c r="D35" s="55"/>
+      <c r="E35" s="55"/>
+      <c r="F35" s="55"/>
+      <c r="G35" s="55"/>
+      <c r="H35" s="55"/>
+      <c r="I35" s="55"/>
+      <c r="J35" s="55"/>
+      <c r="K35" s="56"/>
       <c r="L35" s="27"/>
     </row>
     <row r="36" spans="1:12" x14ac:dyDescent="0.25">
@@ -2228,15 +2228,15 @@
         <v>28</v>
       </c>
       <c r="B36" s="11"/>
-      <c r="C36" s="80"/>
-      <c r="D36" s="80"/>
-      <c r="E36" s="80"/>
-      <c r="F36" s="80"/>
-      <c r="G36" s="80"/>
-      <c r="H36" s="80"/>
-      <c r="I36" s="80"/>
-      <c r="J36" s="80"/>
-      <c r="K36" s="81"/>
+      <c r="C36" s="55"/>
+      <c r="D36" s="55"/>
+      <c r="E36" s="55"/>
+      <c r="F36" s="55"/>
+      <c r="G36" s="55"/>
+      <c r="H36" s="55"/>
+      <c r="I36" s="55"/>
+      <c r="J36" s="55"/>
+      <c r="K36" s="56"/>
       <c r="L36" s="27"/>
     </row>
     <row r="37" spans="1:12" x14ac:dyDescent="0.25">
@@ -2244,15 +2244,15 @@
         <v>29</v>
       </c>
       <c r="B37" s="11"/>
-      <c r="C37" s="80"/>
-      <c r="D37" s="80"/>
-      <c r="E37" s="80"/>
-      <c r="F37" s="80"/>
-      <c r="G37" s="80"/>
-      <c r="H37" s="80"/>
-      <c r="I37" s="80"/>
-      <c r="J37" s="80"/>
-      <c r="K37" s="81"/>
+      <c r="C37" s="55"/>
+      <c r="D37" s="55"/>
+      <c r="E37" s="55"/>
+      <c r="F37" s="55"/>
+      <c r="G37" s="55"/>
+      <c r="H37" s="55"/>
+      <c r="I37" s="55"/>
+      <c r="J37" s="55"/>
+      <c r="K37" s="56"/>
       <c r="L37" s="27"/>
     </row>
     <row r="38" spans="1:12" x14ac:dyDescent="0.25">
@@ -2260,15 +2260,15 @@
         <v>30</v>
       </c>
       <c r="B38" s="11"/>
-      <c r="C38" s="80"/>
-      <c r="D38" s="80"/>
-      <c r="E38" s="80"/>
-      <c r="F38" s="80"/>
-      <c r="G38" s="80"/>
-      <c r="H38" s="80"/>
-      <c r="I38" s="80"/>
-      <c r="J38" s="80"/>
-      <c r="K38" s="81"/>
+      <c r="C38" s="55"/>
+      <c r="D38" s="55"/>
+      <c r="E38" s="55"/>
+      <c r="F38" s="55"/>
+      <c r="G38" s="55"/>
+      <c r="H38" s="55"/>
+      <c r="I38" s="55"/>
+      <c r="J38" s="55"/>
+      <c r="K38" s="56"/>
       <c r="L38" s="27"/>
     </row>
     <row r="39" spans="1:12" x14ac:dyDescent="0.25">
@@ -2276,15 +2276,15 @@
         <v>31</v>
       </c>
       <c r="B39" s="11"/>
-      <c r="C39" s="80"/>
-      <c r="D39" s="80"/>
-      <c r="E39" s="80"/>
-      <c r="F39" s="80"/>
-      <c r="G39" s="80"/>
-      <c r="H39" s="80"/>
-      <c r="I39" s="80"/>
-      <c r="J39" s="80"/>
-      <c r="K39" s="81"/>
+      <c r="C39" s="55"/>
+      <c r="D39" s="55"/>
+      <c r="E39" s="55"/>
+      <c r="F39" s="55"/>
+      <c r="G39" s="55"/>
+      <c r="H39" s="55"/>
+      <c r="I39" s="55"/>
+      <c r="J39" s="55"/>
+      <c r="K39" s="56"/>
       <c r="L39" s="27"/>
     </row>
     <row r="40" spans="1:12" x14ac:dyDescent="0.25">
@@ -2292,17 +2292,17 @@
         <v>33</v>
       </c>
       <c r="B40" s="11"/>
-      <c r="C40" s="80" t="s">
+      <c r="C40" s="55" t="s">
         <v>34</v>
       </c>
-      <c r="D40" s="80"/>
-      <c r="E40" s="80"/>
-      <c r="F40" s="80"/>
-      <c r="G40" s="80"/>
-      <c r="H40" s="80"/>
-      <c r="I40" s="80"/>
-      <c r="J40" s="80"/>
-      <c r="K40" s="81"/>
+      <c r="D40" s="55"/>
+      <c r="E40" s="55"/>
+      <c r="F40" s="55"/>
+      <c r="G40" s="55"/>
+      <c r="H40" s="55"/>
+      <c r="I40" s="55"/>
+      <c r="J40" s="55"/>
+      <c r="K40" s="56"/>
       <c r="L40" s="27"/>
     </row>
     <row r="41" spans="1:12" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -2320,38 +2320,47 @@
       <c r="L41" s="27"/>
     </row>
     <row r="42" spans="1:12" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="90" t="s">
-        <v>55</v>
-      </c>
-      <c r="B42" s="91"/>
-      <c r="C42" s="91"/>
-      <c r="D42" s="91"/>
-      <c r="E42" s="91"/>
-      <c r="F42" s="91"/>
-      <c r="G42" s="91"/>
-      <c r="H42" s="91"/>
-      <c r="I42" s="91"/>
-      <c r="J42" s="91"/>
-      <c r="K42" s="91"/>
+      <c r="A42" s="57" t="s">
+        <v>54</v>
+      </c>
+      <c r="B42" s="58"/>
+      <c r="C42" s="58"/>
+      <c r="D42" s="58"/>
+      <c r="E42" s="58"/>
+      <c r="F42" s="58"/>
+      <c r="G42" s="58"/>
+      <c r="H42" s="58"/>
+      <c r="I42" s="58"/>
+      <c r="J42" s="58"/>
+      <c r="K42" s="58"/>
       <c r="L42" s="27"/>
     </row>
     <row r="43" spans="1:12" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A43" s="92"/>
-      <c r="B43" s="93"/>
-      <c r="C43" s="93"/>
-      <c r="D43" s="93"/>
-      <c r="E43" s="93"/>
-      <c r="F43" s="93"/>
-      <c r="G43" s="93"/>
-      <c r="H43" s="93"/>
-      <c r="I43" s="93"/>
-      <c r="J43" s="93"/>
-      <c r="K43" s="93"/>
+      <c r="A43" s="59"/>
+      <c r="B43" s="60"/>
+      <c r="C43" s="60"/>
+      <c r="D43" s="60"/>
+      <c r="E43" s="60"/>
+      <c r="F43" s="60"/>
+      <c r="G43" s="60"/>
+      <c r="H43" s="60"/>
+      <c r="I43" s="60"/>
+      <c r="J43" s="60"/>
+      <c r="K43" s="60"/>
       <c r="L43" s="33"/>
     </row>
     <row r="44" spans="1:12" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="25">
+    <mergeCell ref="C25:K25"/>
+    <mergeCell ref="C6:K6"/>
+    <mergeCell ref="C14:K14"/>
+    <mergeCell ref="C15:K15"/>
+    <mergeCell ref="A1:K4"/>
+    <mergeCell ref="C7:K8"/>
+    <mergeCell ref="C11:K11"/>
+    <mergeCell ref="C20:K20"/>
+    <mergeCell ref="C21:K21"/>
     <mergeCell ref="C12:K13"/>
     <mergeCell ref="C40:K40"/>
     <mergeCell ref="A42:K43"/>
@@ -2365,18 +2374,9 @@
     <mergeCell ref="C17:K17"/>
     <mergeCell ref="C19:K19"/>
     <mergeCell ref="C27:K27"/>
-    <mergeCell ref="A1:K4"/>
-    <mergeCell ref="C7:K8"/>
-    <mergeCell ref="C11:K11"/>
-    <mergeCell ref="C20:K20"/>
-    <mergeCell ref="C21:K21"/>
     <mergeCell ref="C22:K22"/>
     <mergeCell ref="C23:K23"/>
     <mergeCell ref="C24:K24"/>
-    <mergeCell ref="C25:K25"/>
-    <mergeCell ref="C6:K6"/>
-    <mergeCell ref="C14:K14"/>
-    <mergeCell ref="C15:K15"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>

</xml_diff>